<commit_message>
Corrigido teste de ativo/passivo intra para desconsiderar o PL.
</commit_message>
<xml_diff>
--- a/report-cm.xlsx
+++ b/report-cm.xlsx
@@ -538,7 +538,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>3693304.18</v>
+        <v>4734802.97</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -577,7 +577,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>2999071.75</v>
+        <v>3220092.88</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -616,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1106028.25</v>
+        <v>1485738.41</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -700,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>2150044.72</v>
+        <v>3053815.92</v>
       </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>3012253.3</v>
+        <v>3260420.17</v>
       </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>2645678.66</v>
+        <v>3135970.67</v>
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
@@ -837,7 +837,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
-        <v>7810404.18</v>
+        <v>9452634.26</v>
       </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
@@ -845,7 +845,7 @@
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
-        <v>7810404.18</v>
+        <v>9452634.26</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>2498265.37</v>
+        <v>2698679.53</v>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
@@ -918,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>2303103.21</v>
+        <v>3344083.67</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
@@ -963,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>28203.09</v>
+        <v>28272.99</v>
       </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -1002,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>4773165.49</v>
+        <v>6014490.21</v>
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
@@ -1022,7 +1022,7 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
-        <v>4801368.58</v>
+        <v>6042763.199999999</v>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
@@ -1030,10 +1030,10 @@
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
-        <v>4801368.58</v>
+        <v>6042763.2</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="16">
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>1024673.46</v>
+        <v>1351897.6</v>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>1407633.63</v>
+        <v>2034462.54</v>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>2420922.19</v>
+        <v>3374975.24</v>
       </c>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
@@ -1207,7 +1207,7 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
-        <v>2432307.09</v>
+        <v>3386360.14</v>
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
@@ -1215,7 +1215,7 @@
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="n">
-        <v>2432307.09</v>
+        <v>3386360.14</v>
       </c>
       <c r="O20" t="n">
         <v>0</v>
@@ -2038,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>2802.72</v>
+        <v>3028.45</v>
       </c>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
@@ -2122,7 +2122,7 @@
         <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>2802.72</v>
+        <v>3028.45</v>
       </c>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr"/>
@@ -2142,7 +2142,7 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
-        <v>2802.72</v>
+        <v>3028.45</v>
       </c>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr"/>
@@ -2150,7 +2150,7 @@
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="n">
-        <v>2802.72</v>
+        <v>3028.45</v>
       </c>
       <c r="O45" t="n">
         <v>0</v>
@@ -2268,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="M48" t="n">
-        <v>54761.81</v>
+        <v>76130.23</v>
       </c>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
@@ -2307,7 +2307,7 @@
         <v>1</v>
       </c>
       <c r="M49" t="n">
-        <v>-44077.6</v>
+        <v>-65446.02</v>
       </c>
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr"/>
@@ -3846,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>486880.47</v>
+        <v>687294.63</v>
       </c>
       <c r="H92" t="inlineStr"/>
       <c r="I92" t="inlineStr"/>
@@ -3885,7 +3885,7 @@
         <v>1</v>
       </c>
       <c r="G93" t="n">
-        <v>-4818.19</v>
+        <v>-4888.09</v>
       </c>
       <c r="H93" t="inlineStr"/>
       <c r="I93" t="inlineStr"/>
@@ -3926,7 +3926,7 @@
         <v>0</v>
       </c>
       <c r="M94" t="n">
-        <v>482062.28</v>
+        <v>682406.54</v>
       </c>
       <c r="N94" t="inlineStr"/>
       <c r="O94" t="inlineStr"/>
@@ -3946,7 +3946,7 @@
       <c r="F95" t="inlineStr"/>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="n">
-        <v>482062.28</v>
+        <v>682406.54</v>
       </c>
       <c r="I95" t="inlineStr"/>
       <c r="J95" t="inlineStr"/>
@@ -3954,10 +3954,10 @@
       <c r="L95" t="inlineStr"/>
       <c r="M95" t="inlineStr"/>
       <c r="N95" t="n">
-        <v>482062.28</v>
+        <v>682406.54</v>
       </c>
       <c r="O95" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -5124,7 +5124,7 @@
         <v>0</v>
       </c>
       <c r="G128" t="n">
-        <v>36550.48</v>
+        <v>19649.41</v>
       </c>
       <c r="H128" t="inlineStr"/>
       <c r="I128" t="inlineStr"/>
@@ -5204,7 +5204,7 @@
         <v>0</v>
       </c>
       <c r="M130" t="n">
-        <v>482062.28</v>
+        <v>682406.54</v>
       </c>
       <c r="N130" t="inlineStr"/>
       <c r="O130" t="inlineStr"/>
@@ -5239,7 +5239,7 @@
         <v>1</v>
       </c>
       <c r="M131" t="n">
-        <v>-445511.8</v>
+        <v>-662757.13</v>
       </c>
       <c r="N131" t="inlineStr"/>
       <c r="O131" t="inlineStr"/>
@@ -5259,7 +5259,7 @@
       <c r="F132" t="inlineStr"/>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="n">
-        <v>36550.48</v>
+        <v>19649.41</v>
       </c>
       <c r="I132" t="inlineStr"/>
       <c r="J132" t="inlineStr"/>
@@ -5267,7 +5267,7 @@
       <c r="L132" t="inlineStr"/>
       <c r="M132" t="inlineStr"/>
       <c r="N132" t="n">
-        <v>36550.48000000004</v>
+        <v>19649.41000000003</v>
       </c>
       <c r="O132" t="n">
         <v>-0</v>
@@ -5301,7 +5301,7 @@
         <v>0</v>
       </c>
       <c r="G133" t="n">
-        <v>36550.48</v>
+        <v>19649.41</v>
       </c>
       <c r="H133" t="inlineStr"/>
       <c r="I133" t="inlineStr"/>
@@ -5381,7 +5381,7 @@
         <v>0</v>
       </c>
       <c r="M135" t="n">
-        <v>482062.28</v>
+        <v>682406.54</v>
       </c>
       <c r="N135" t="inlineStr"/>
       <c r="O135" t="inlineStr"/>
@@ -5416,7 +5416,7 @@
         <v>1</v>
       </c>
       <c r="M136" t="n">
-        <v>-445511.8</v>
+        <v>-662757.13</v>
       </c>
       <c r="N136" t="inlineStr"/>
       <c r="O136" t="inlineStr"/>
@@ -5436,7 +5436,7 @@
       <c r="F137" t="inlineStr"/>
       <c r="G137" t="inlineStr"/>
       <c r="H137" t="n">
-        <v>36550.48</v>
+        <v>19649.41</v>
       </c>
       <c r="I137" t="inlineStr"/>
       <c r="J137" t="inlineStr"/>
@@ -5444,7 +5444,7 @@
       <c r="L137" t="inlineStr"/>
       <c r="M137" t="inlineStr"/>
       <c r="N137" t="n">
-        <v>36550.48000000004</v>
+        <v>19649.41000000003</v>
       </c>
       <c r="O137" t="n">
         <v>-0</v>
@@ -5478,7 +5478,7 @@
         <v>0</v>
       </c>
       <c r="G138" t="n">
-        <v>15610.32</v>
+        <v>29887.73</v>
       </c>
       <c r="H138" t="inlineStr"/>
       <c r="I138" t="inlineStr"/>
@@ -5558,7 +5558,7 @@
         <v>0</v>
       </c>
       <c r="M140" t="n">
-        <v>445511.8</v>
+        <v>662757.13</v>
       </c>
       <c r="N140" t="inlineStr"/>
       <c r="O140" t="inlineStr"/>
@@ -5593,7 +5593,7 @@
         <v>1</v>
       </c>
       <c r="M141" t="n">
-        <v>-429901.48</v>
+        <v>-632869.4</v>
       </c>
       <c r="N141" t="inlineStr"/>
       <c r="O141" t="inlineStr"/>
@@ -5613,7 +5613,7 @@
       <c r="F142" t="inlineStr"/>
       <c r="G142" t="inlineStr"/>
       <c r="H142" t="n">
-        <v>15610.32</v>
+        <v>29887.73</v>
       </c>
       <c r="I142" t="inlineStr"/>
       <c r="J142" t="inlineStr"/>
@@ -5621,10 +5621,10 @@
       <c r="L142" t="inlineStr"/>
       <c r="M142" t="inlineStr"/>
       <c r="N142" t="n">
-        <v>15610.32000000001</v>
+        <v>29887.72999999998</v>
       </c>
       <c r="O142" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -5655,7 +5655,7 @@
         <v>0</v>
       </c>
       <c r="G143" t="n">
-        <v>15610.32</v>
+        <v>29887.73</v>
       </c>
       <c r="H143" t="inlineStr"/>
       <c r="I143" t="inlineStr"/>
@@ -5735,7 +5735,7 @@
         <v>0</v>
       </c>
       <c r="M145" t="n">
-        <v>445511.8</v>
+        <v>662757.13</v>
       </c>
       <c r="N145" t="inlineStr"/>
       <c r="O145" t="inlineStr"/>
@@ -5770,7 +5770,7 @@
         <v>1</v>
       </c>
       <c r="M146" t="n">
-        <v>-429901.48</v>
+        <v>-632869.4</v>
       </c>
       <c r="N146" t="inlineStr"/>
       <c r="O146" t="inlineStr"/>
@@ -5790,7 +5790,7 @@
       <c r="F147" t="inlineStr"/>
       <c r="G147" t="inlineStr"/>
       <c r="H147" t="n">
-        <v>15610.32</v>
+        <v>29887.73</v>
       </c>
       <c r="I147" t="inlineStr"/>
       <c r="J147" t="inlineStr"/>
@@ -5798,10 +5798,10 @@
       <c r="L147" t="inlineStr"/>
       <c r="M147" t="inlineStr"/>
       <c r="N147" t="n">
-        <v>15610.32000000001</v>
+        <v>29887.72999999998</v>
       </c>
       <c r="O147" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -5832,7 +5832,7 @@
         <v>0</v>
       </c>
       <c r="G148" t="n">
-        <v>429901.48</v>
+        <v>632869.4</v>
       </c>
       <c r="H148" t="inlineStr"/>
       <c r="I148" t="inlineStr"/>
@@ -5912,7 +5912,7 @@
         <v>0</v>
       </c>
       <c r="M150" t="n">
-        <v>429901.48</v>
+        <v>632869.4</v>
       </c>
       <c r="N150" t="inlineStr"/>
       <c r="O150" t="inlineStr"/>
@@ -5932,7 +5932,7 @@
       <c r="F151" t="inlineStr"/>
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="n">
-        <v>429901.48</v>
+        <v>632869.4</v>
       </c>
       <c r="I151" t="inlineStr"/>
       <c r="J151" t="inlineStr"/>
@@ -5940,7 +5940,7 @@
       <c r="L151" t="inlineStr"/>
       <c r="M151" t="inlineStr"/>
       <c r="N151" t="n">
-        <v>429901.48</v>
+        <v>632869.4</v>
       </c>
       <c r="O151" t="n">
         <v>0</v>
@@ -5974,7 +5974,7 @@
         <v>0</v>
       </c>
       <c r="G152" t="n">
-        <v>429901.48</v>
+        <v>632869.4</v>
       </c>
       <c r="H152" t="inlineStr"/>
       <c r="I152" t="inlineStr"/>
@@ -6054,7 +6054,7 @@
         <v>0</v>
       </c>
       <c r="M154" t="n">
-        <v>429901.48</v>
+        <v>632869.4</v>
       </c>
       <c r="N154" t="inlineStr"/>
       <c r="O154" t="inlineStr"/>
@@ -6074,7 +6074,7 @@
       <c r="F155" t="inlineStr"/>
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="n">
-        <v>429901.48</v>
+        <v>632869.4</v>
       </c>
       <c r="I155" t="inlineStr"/>
       <c r="J155" t="inlineStr"/>
@@ -6082,7 +6082,7 @@
       <c r="L155" t="inlineStr"/>
       <c r="M155" t="inlineStr"/>
       <c r="N155" t="n">
-        <v>429901.48</v>
+        <v>632869.4</v>
       </c>
       <c r="O155" t="n">
         <v>0</v>
@@ -8078,7 +8078,7 @@
         <v>0</v>
       </c>
       <c r="G210" t="n">
-        <v>486880.47</v>
+        <v>687294.63</v>
       </c>
       <c r="H210" t="inlineStr"/>
       <c r="I210" t="inlineStr"/>
@@ -8117,7 +8117,7 @@
         <v>1</v>
       </c>
       <c r="G211" t="n">
-        <v>-4818.19</v>
+        <v>-4888.09</v>
       </c>
       <c r="H211" t="inlineStr"/>
       <c r="I211" t="inlineStr"/>
@@ -8162,7 +8162,7 @@
         <v>0</v>
       </c>
       <c r="M212" t="n">
-        <v>482062.28</v>
+        <v>682406.54</v>
       </c>
       <c r="N212" t="inlineStr"/>
       <c r="O212" t="inlineStr"/>
@@ -8221,7 +8221,7 @@
       <c r="F214" t="inlineStr"/>
       <c r="G214" t="inlineStr"/>
       <c r="H214" t="n">
-        <v>482062.28</v>
+        <v>682406.54</v>
       </c>
       <c r="I214" t="inlineStr"/>
       <c r="J214" t="inlineStr"/>
@@ -8229,10 +8229,10 @@
       <c r="L214" t="inlineStr"/>
       <c r="M214" t="inlineStr"/>
       <c r="N214" t="n">
-        <v>482062.28</v>
+        <v>682406.54</v>
       </c>
       <c r="O214" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215">
@@ -24913,7 +24913,7 @@
         <v>0</v>
       </c>
       <c r="G665" t="n">
-        <v>657331.04</v>
+        <v>984309.72</v>
       </c>
       <c r="H665" t="inlineStr"/>
       <c r="I665" t="inlineStr"/>
@@ -24997,7 +24997,7 @@
         <v>0</v>
       </c>
       <c r="M667" t="n">
-        <v>657331.04</v>
+        <v>984309.72</v>
       </c>
       <c r="N667" t="inlineStr"/>
       <c r="O667" t="inlineStr"/>
@@ -25056,7 +25056,7 @@
       <c r="F669" t="inlineStr"/>
       <c r="G669" t="inlineStr"/>
       <c r="H669" t="n">
-        <v>657331.04</v>
+        <v>984309.72</v>
       </c>
       <c r="I669" t="inlineStr"/>
       <c r="J669" t="inlineStr"/>
@@ -25064,7 +25064,7 @@
       <c r="L669" t="inlineStr"/>
       <c r="M669" t="inlineStr"/>
       <c r="N669" t="n">
-        <v>657331.04</v>
+        <v>984309.72</v>
       </c>
       <c r="O669" t="n">
         <v>0</v>
@@ -33608,7 +33608,7 @@
         <v>0</v>
       </c>
       <c r="G900" t="n">
-        <v>181.3</v>
+        <v>426.76</v>
       </c>
       <c r="H900" t="inlineStr"/>
       <c r="I900" t="inlineStr"/>
@@ -33692,7 +33692,7 @@
         <v>0</v>
       </c>
       <c r="M902" t="n">
-        <v>181.3</v>
+        <v>426.76</v>
       </c>
       <c r="N902" t="inlineStr"/>
       <c r="O902" t="inlineStr"/>
@@ -33751,7 +33751,7 @@
       <c r="F904" t="inlineStr"/>
       <c r="G904" t="inlineStr"/>
       <c r="H904" t="n">
-        <v>181.3</v>
+        <v>426.76</v>
       </c>
       <c r="I904" t="inlineStr"/>
       <c r="J904" t="inlineStr"/>
@@ -33759,7 +33759,7 @@
       <c r="L904" t="inlineStr"/>
       <c r="M904" t="inlineStr"/>
       <c r="N904" t="n">
-        <v>181.3</v>
+        <v>426.76</v>
       </c>
       <c r="O904" t="n">
         <v>0</v>
@@ -34533,7 +34533,7 @@
         <v>0</v>
       </c>
       <c r="G925" t="n">
-        <v>657331.04</v>
+        <v>984309.72</v>
       </c>
       <c r="H925" t="inlineStr"/>
       <c r="I925" t="inlineStr"/>
@@ -34611,7 +34611,7 @@
         <v>1</v>
       </c>
       <c r="G927" t="n">
-        <v>-441553.86</v>
+        <v>-644687.5600000001</v>
       </c>
       <c r="H927" t="inlineStr"/>
       <c r="I927" t="inlineStr"/>
@@ -34695,7 +34695,7 @@
         <v>0</v>
       </c>
       <c r="M929" t="n">
-        <v>215777.18</v>
+        <v>339622.16</v>
       </c>
       <c r="N929" t="inlineStr"/>
       <c r="O929" t="inlineStr"/>
@@ -34832,7 +34832,7 @@
       <c r="F933" t="inlineStr"/>
       <c r="G933" t="inlineStr"/>
       <c r="H933" t="n">
-        <v>215777.1800000001</v>
+        <v>339622.1599999999</v>
       </c>
       <c r="I933" t="inlineStr"/>
       <c r="J933" t="inlineStr"/>
@@ -34840,10 +34840,10 @@
       <c r="L933" t="inlineStr"/>
       <c r="M933" t="inlineStr"/>
       <c r="N933" t="n">
-        <v>215777.18</v>
+        <v>339622.16</v>
       </c>
       <c r="O933" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="934">
@@ -34874,7 +34874,7 @@
         <v>0</v>
       </c>
       <c r="G934" t="n">
-        <v>163616.38</v>
+        <v>290085.02</v>
       </c>
       <c r="H934" t="inlineStr"/>
       <c r="I934" t="inlineStr"/>
@@ -34958,7 +34958,7 @@
         <v>0</v>
       </c>
       <c r="M936" t="n">
-        <v>215777.18</v>
+        <v>339622.16</v>
       </c>
       <c r="N936" t="inlineStr"/>
       <c r="O936" t="inlineStr"/>
@@ -35036,7 +35036,7 @@
         <v>1</v>
       </c>
       <c r="M938" t="n">
-        <v>-15610.32</v>
+        <v>-29887.73</v>
       </c>
       <c r="N938" t="inlineStr"/>
       <c r="O938" t="inlineStr"/>
@@ -35192,7 +35192,7 @@
         <v>1</v>
       </c>
       <c r="M942" t="n">
-        <v>-36550.48</v>
+        <v>-19649.41</v>
       </c>
       <c r="N942" t="inlineStr"/>
       <c r="O942" t="inlineStr"/>
@@ -35251,7 +35251,7 @@
       <c r="F944" t="inlineStr"/>
       <c r="G944" t="inlineStr"/>
       <c r="H944" t="n">
-        <v>163616.38</v>
+        <v>290085.02</v>
       </c>
       <c r="I944" t="inlineStr"/>
       <c r="J944" t="inlineStr"/>
@@ -35259,7 +35259,7 @@
       <c r="L944" t="inlineStr"/>
       <c r="M944" t="inlineStr"/>
       <c r="N944" t="n">
-        <v>163616.38</v>
+        <v>290085.02</v>
       </c>
       <c r="O944" t="n">
         <v>0</v>
@@ -35293,7 +35293,7 @@
         <v>0</v>
       </c>
       <c r="G945" t="n">
-        <v>1677633.89</v>
+        <v>1817134.5</v>
       </c>
       <c r="H945" t="inlineStr"/>
       <c r="I945" t="inlineStr"/>
@@ -35332,7 +35332,7 @@
         <v>1</v>
       </c>
       <c r="G946" t="n">
-        <v>-49246.63</v>
+        <v>-51019.65</v>
       </c>
       <c r="H946" t="inlineStr"/>
       <c r="I946" t="inlineStr"/>
@@ -35410,7 +35410,7 @@
         <v>1</v>
       </c>
       <c r="G948" t="n">
-        <v>-2279453.2</v>
+        <v>-2306598.94</v>
       </c>
       <c r="H948" t="inlineStr"/>
       <c r="I948" t="inlineStr"/>
@@ -35455,7 +35455,7 @@
         <v>0</v>
       </c>
       <c r="M949" t="n">
-        <v>2633678.66</v>
+        <v>3123970.67</v>
       </c>
       <c r="N949" t="inlineStr"/>
       <c r="O949" t="inlineStr"/>
@@ -35572,7 +35572,7 @@
         <v>1</v>
       </c>
       <c r="M952" t="n">
-        <v>-1103600.75</v>
+        <v>-1483310.91</v>
       </c>
       <c r="N952" t="inlineStr"/>
       <c r="O952" t="inlineStr"/>
@@ -35592,7 +35592,7 @@
       <c r="F953" t="inlineStr"/>
       <c r="G953" t="inlineStr"/>
       <c r="H953" t="n">
-        <v>1530077.91</v>
+        <v>1640659.76</v>
       </c>
       <c r="I953" t="inlineStr"/>
       <c r="J953" t="inlineStr"/>
@@ -35600,7 +35600,7 @@
       <c r="L953" t="inlineStr"/>
       <c r="M953" t="inlineStr"/>
       <c r="N953" t="n">
-        <v>1530077.91</v>
+        <v>1640659.76</v>
       </c>
       <c r="O953" t="n">
         <v>0</v>
@@ -35634,7 +35634,7 @@
         <v>0</v>
       </c>
       <c r="G954" t="n">
-        <v>163616.38</v>
+        <v>290085.02</v>
       </c>
       <c r="H954" t="inlineStr"/>
       <c r="I954" t="inlineStr"/>
@@ -36030,7 +36030,7 @@
         <v>0</v>
       </c>
       <c r="M964" t="n">
-        <v>645678.66</v>
+        <v>972491.5600000001</v>
       </c>
       <c r="N964" t="inlineStr"/>
       <c r="O964" t="inlineStr"/>
@@ -36221,7 +36221,7 @@
         <v>1</v>
       </c>
       <c r="M969" t="n">
-        <v>-482062.28</v>
+        <v>-682406.54</v>
       </c>
       <c r="N969" t="inlineStr"/>
       <c r="O969" t="inlineStr"/>
@@ -36545,7 +36545,7 @@
       <c r="F978" t="inlineStr"/>
       <c r="G978" t="inlineStr"/>
       <c r="H978" t="n">
-        <v>163616.38</v>
+        <v>290085.02</v>
       </c>
       <c r="I978" t="inlineStr"/>
       <c r="J978" t="inlineStr"/>
@@ -36553,7 +36553,7 @@
       <c r="L978" t="inlineStr"/>
       <c r="M978" t="inlineStr"/>
       <c r="N978" t="n">
-        <v>163616.38</v>
+        <v>290085.02</v>
       </c>
       <c r="O978" t="n">
         <v>0</v>
@@ -36587,7 +36587,7 @@
         <v>0</v>
       </c>
       <c r="G979" t="n">
-        <v>163616.38</v>
+        <v>290085.02</v>
       </c>
       <c r="H979" t="inlineStr"/>
       <c r="I979" t="inlineStr"/>
@@ -36671,7 +36671,7 @@
         <v>0</v>
       </c>
       <c r="M981" t="n">
-        <v>215777.18</v>
+        <v>339622.16</v>
       </c>
       <c r="N981" t="inlineStr"/>
       <c r="O981" t="inlineStr"/>
@@ -36749,7 +36749,7 @@
         <v>1</v>
       </c>
       <c r="M983" t="n">
-        <v>-15610.32</v>
+        <v>-29887.73</v>
       </c>
       <c r="N983" t="inlineStr"/>
       <c r="O983" t="inlineStr"/>
@@ -36905,7 +36905,7 @@
         <v>1</v>
       </c>
       <c r="M987" t="n">
-        <v>-36550.48</v>
+        <v>-19649.41</v>
       </c>
       <c r="N987" t="inlineStr"/>
       <c r="O987" t="inlineStr"/>
@@ -36964,7 +36964,7 @@
       <c r="F989" t="inlineStr"/>
       <c r="G989" t="inlineStr"/>
       <c r="H989" t="n">
-        <v>163616.38</v>
+        <v>290085.02</v>
       </c>
       <c r="I989" t="inlineStr"/>
       <c r="J989" t="inlineStr"/>
@@ -36972,7 +36972,7 @@
       <c r="L989" t="inlineStr"/>
       <c r="M989" t="inlineStr"/>
       <c r="N989" t="n">
-        <v>163616.38</v>
+        <v>290085.02</v>
       </c>
       <c r="O989" t="n">
         <v>0</v>
@@ -37006,7 +37006,7 @@
         <v>0</v>
       </c>
       <c r="G990" t="n">
-        <v>36550.48</v>
+        <v>19649.41</v>
       </c>
       <c r="H990" t="inlineStr"/>
       <c r="I990" t="inlineStr"/>
@@ -37090,7 +37090,7 @@
         <v>0</v>
       </c>
       <c r="M992" t="n">
-        <v>36550.48</v>
+        <v>19649.41</v>
       </c>
       <c r="N992" t="inlineStr"/>
       <c r="O992" t="inlineStr"/>
@@ -37227,7 +37227,7 @@
       <c r="F996" t="inlineStr"/>
       <c r="G996" t="inlineStr"/>
       <c r="H996" t="n">
-        <v>36550.48</v>
+        <v>19649.41</v>
       </c>
       <c r="I996" t="inlineStr"/>
       <c r="J996" t="inlineStr"/>
@@ -37235,7 +37235,7 @@
       <c r="L996" t="inlineStr"/>
       <c r="M996" t="inlineStr"/>
       <c r="N996" t="n">
-        <v>36550.48</v>
+        <v>19649.41</v>
       </c>
       <c r="O996" t="n">
         <v>0</v>
@@ -37269,7 +37269,7 @@
         <v>0</v>
       </c>
       <c r="G997" t="n">
-        <v>15610.32</v>
+        <v>29887.73</v>
       </c>
       <c r="H997" t="inlineStr"/>
       <c r="I997" t="inlineStr"/>
@@ -37353,7 +37353,7 @@
         <v>0</v>
       </c>
       <c r="M999" t="n">
-        <v>15610.32</v>
+        <v>29887.73</v>
       </c>
       <c r="N999" t="inlineStr"/>
       <c r="O999" t="inlineStr"/>
@@ -37724,7 +37724,7 @@
       <c r="F1009" t="inlineStr"/>
       <c r="G1009" t="inlineStr"/>
       <c r="H1009" t="n">
-        <v>15610.32</v>
+        <v>29887.73</v>
       </c>
       <c r="I1009" t="inlineStr"/>
       <c r="J1009" t="inlineStr"/>
@@ -37732,7 +37732,7 @@
       <c r="L1009" t="inlineStr"/>
       <c r="M1009" t="inlineStr"/>
       <c r="N1009" t="n">
-        <v>15610.32</v>
+        <v>29887.73</v>
       </c>
       <c r="O1009" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Modificados caminhos para usar OneDrive.
</commit_message>
<xml_diff>
--- a/report-cm.xlsx
+++ b/report-cm.xlsx
@@ -538,7 +538,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>5589871.8</v>
+        <v>3499702.23</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -577,7 +577,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>3424393.85</v>
+        <v>2815927.88</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -616,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>2011588.29</v>
+        <v>614120.74</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -655,7 +655,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>12000</v>
+        <v>0</v>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
@@ -700,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>4069805.81</v>
+        <v>1191837.85</v>
       </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>3463748.38</v>
+        <v>2825613.44</v>
       </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
@@ -778,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>2427.5</v>
+        <v>0</v>
       </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>3501872.25</v>
+        <v>2912299.56</v>
       </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
@@ -837,7 +837,7 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
-        <v>11037853.94</v>
+        <v>6929750.85</v>
       </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
@@ -845,7 +845,7 @@
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
-        <v>11037853.94</v>
+        <v>6929750.85</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>2927197.03</v>
+        <v>2743149.86</v>
       </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
@@ -918,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>4312783.57</v>
+        <v>1016282.22</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
@@ -963,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>71969.83</v>
+        <v>0</v>
       </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
@@ -1002,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>7168010.77</v>
+        <v>3759432.08</v>
       </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
@@ -1022,7 +1022,7 @@
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
-        <v>7239980.6</v>
+        <v>3759432.08</v>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
@@ -1030,7 +1030,7 @@
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
-        <v>7239980.6</v>
+        <v>3759432.08</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>1696439.58</v>
+        <v>413341.85</v>
       </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>2912872.82</v>
+        <v>638203.33</v>
       </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>311384.9</v>
+        <v>0</v>
       </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>4297927.5</v>
+        <v>1051545.18</v>
       </c>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
@@ -1207,7 +1207,7 @@
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
-        <v>4609312.4</v>
+        <v>1051545.18</v>
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
@@ -1215,7 +1215,7 @@
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="n">
-        <v>4609312.4</v>
+        <v>1051545.18</v>
       </c>
       <c r="O20" t="n">
         <v>0</v>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>conta_contabil like "8129101%" and escrituracao like "S"</t>
+          <t>conta_contabil like "8990001%" and escrituracao like "S"</t>
         </is>
       </c>
       <c r="L39" t="b">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>conta_contabil like "8129101%" and escrituracao like "S"</t>
+          <t>conta_contabil like "8990001%" and escrituracao like "S"</t>
         </is>
       </c>
       <c r="L40" t="b">
@@ -2038,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>1109.78</v>
+        <v>1187.17</v>
       </c>
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
@@ -2122,7 +2122,7 @@
         <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>1109.78</v>
+        <v>1187.17</v>
       </c>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr"/>
@@ -2142,7 +2142,7 @@
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
-        <v>1109.78</v>
+        <v>1187.17</v>
       </c>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr"/>
@@ -2150,7 +2150,7 @@
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="n">
-        <v>1109.78</v>
+        <v>1187.17</v>
       </c>
       <c r="O45" t="n">
         <v>0</v>
@@ -2184,7 +2184,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>10979.18</v>
+        <v>4931</v>
       </c>
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="inlineStr"/>
@@ -2268,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="M48" t="n">
-        <v>98088.59</v>
+        <v>10921.92</v>
       </c>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
@@ -2307,7 +2307,7 @@
         <v>1</v>
       </c>
       <c r="M49" t="n">
-        <v>-87109.41</v>
+        <v>-5990.92</v>
       </c>
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr"/>
@@ -2483,7 +2483,7 @@
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
-        <v>10979.18</v>
+        <v>4931</v>
       </c>
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr"/>
@@ -2491,7 +2491,7 @@
       <c r="L54" t="inlineStr"/>
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="n">
-        <v>10979.17999999999</v>
+        <v>4931</v>
       </c>
       <c r="O54" t="n">
         <v>0</v>
@@ -3214,7 +3214,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>2000000</v>
+        <v>2499000</v>
       </c>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr"/>
@@ -3294,7 +3294,7 @@
         <v>0</v>
       </c>
       <c r="M76" t="n">
-        <v>2000000</v>
+        <v>2499000</v>
       </c>
       <c r="N76" t="inlineStr"/>
       <c r="O76" t="inlineStr"/>
@@ -3314,7 +3314,7 @@
       <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="n">
-        <v>2000000</v>
+        <v>2499000</v>
       </c>
       <c r="I77" t="inlineStr"/>
       <c r="J77" t="inlineStr"/>
@@ -3322,7 +3322,7 @@
       <c r="L77" t="inlineStr"/>
       <c r="M77" t="inlineStr"/>
       <c r="N77" t="n">
-        <v>2000000</v>
+        <v>2499000</v>
       </c>
       <c r="O77" t="n">
         <v>0</v>
@@ -3356,7 +3356,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="H78" t="inlineStr"/>
       <c r="I78" t="inlineStr"/>
@@ -3436,7 +3436,7 @@
         <v>0</v>
       </c>
       <c r="M80" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="N80" t="inlineStr"/>
       <c r="O80" t="inlineStr"/>
@@ -3456,7 +3456,7 @@
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="I81" t="inlineStr"/>
       <c r="J81" t="inlineStr"/>
@@ -3464,7 +3464,7 @@
       <c r="L81" t="inlineStr"/>
       <c r="M81" t="inlineStr"/>
       <c r="N81" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="O81" t="n">
         <v>0</v>
@@ -3821,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>32000</v>
+        <v>0</v>
       </c>
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="inlineStr"/>
@@ -3862,7 +3862,7 @@
         <v>0</v>
       </c>
       <c r="M92" t="n">
-        <v>32000</v>
+        <v>0</v>
       </c>
       <c r="N92" t="inlineStr"/>
       <c r="O92" t="inlineStr"/>
@@ -3882,7 +3882,7 @@
       <c r="F93" t="inlineStr"/>
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="n">
-        <v>32000</v>
+        <v>0</v>
       </c>
       <c r="I93" t="inlineStr"/>
       <c r="J93" t="inlineStr"/>
@@ -3890,7 +3890,7 @@
       <c r="L93" t="inlineStr"/>
       <c r="M93" t="inlineStr"/>
       <c r="N93" t="n">
-        <v>32000</v>
+        <v>0</v>
       </c>
       <c r="O93" t="n">
         <v>0</v>
@@ -3924,7 +3924,7 @@
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>875812.13</v>
+        <v>244149.86</v>
       </c>
       <c r="H94" t="inlineStr"/>
       <c r="I94" t="inlineStr"/>
@@ -3963,7 +3963,7 @@
         <v>1</v>
       </c>
       <c r="G95" t="n">
-        <v>-8584.93</v>
+        <v>-0</v>
       </c>
       <c r="H95" t="inlineStr"/>
       <c r="I95" t="inlineStr"/>
@@ -4004,7 +4004,7 @@
         <v>0</v>
       </c>
       <c r="M96" t="n">
-        <v>867227.2</v>
+        <v>244149.86</v>
       </c>
       <c r="N96" t="inlineStr"/>
       <c r="O96" t="inlineStr"/>
@@ -4024,7 +4024,7 @@
       <c r="F97" t="inlineStr"/>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="n">
-        <v>867227.2</v>
+        <v>244149.86</v>
       </c>
       <c r="I97" t="inlineStr"/>
       <c r="J97" t="inlineStr"/>
@@ -4032,7 +4032,7 @@
       <c r="L97" t="inlineStr"/>
       <c r="M97" t="inlineStr"/>
       <c r="N97" t="n">
-        <v>867227.2</v>
+        <v>244149.86</v>
       </c>
       <c r="O97" t="n">
         <v>0</v>
@@ -4066,7 +4066,7 @@
         <v>0</v>
       </c>
       <c r="G98" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="inlineStr"/>
@@ -4146,7 +4146,7 @@
         <v>0</v>
       </c>
       <c r="M100" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="N100" t="inlineStr"/>
       <c r="O100" t="inlineStr"/>
@@ -4166,7 +4166,7 @@
       <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr"/>
@@ -4174,7 +4174,7 @@
       <c r="L101" t="inlineStr"/>
       <c r="M101" t="inlineStr"/>
       <c r="N101" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="O101" t="n">
         <v>0</v>
@@ -4350,7 +4350,7 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="H106" t="inlineStr"/>
       <c r="I106" t="inlineStr"/>
@@ -4430,7 +4430,7 @@
         <v>0</v>
       </c>
       <c r="M108" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="N108" t="inlineStr"/>
       <c r="O108" t="inlineStr"/>
@@ -4450,7 +4450,7 @@
       <c r="F109" t="inlineStr"/>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="I109" t="inlineStr"/>
       <c r="J109" t="inlineStr"/>
@@ -4458,7 +4458,7 @@
       <c r="L109" t="inlineStr"/>
       <c r="M109" t="inlineStr"/>
       <c r="N109" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="O109" t="n">
         <v>0</v>
@@ -4531,7 +4531,7 @@
         <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="H111" t="inlineStr"/>
       <c r="I111" t="inlineStr"/>
@@ -4572,7 +4572,7 @@
         <v>0</v>
       </c>
       <c r="M112" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="N112" t="inlineStr"/>
       <c r="O112" t="inlineStr"/>
@@ -4592,7 +4592,7 @@
       <c r="F113" t="inlineStr"/>
       <c r="G113" t="inlineStr"/>
       <c r="H113" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="I113" t="inlineStr"/>
       <c r="J113" t="inlineStr"/>
@@ -4600,7 +4600,7 @@
       <c r="L113" t="inlineStr"/>
       <c r="M113" t="inlineStr"/>
       <c r="N113" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="O113" t="n">
         <v>0</v>
@@ -4634,7 +4634,7 @@
         <v>0</v>
       </c>
       <c r="G114" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="H114" t="inlineStr"/>
       <c r="I114" t="inlineStr"/>
@@ -4714,7 +4714,7 @@
         <v>0</v>
       </c>
       <c r="M116" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="N116" t="inlineStr"/>
       <c r="O116" t="inlineStr"/>
@@ -4734,7 +4734,7 @@
       <c r="F117" t="inlineStr"/>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr"/>
@@ -4742,7 +4742,7 @@
       <c r="L117" t="inlineStr"/>
       <c r="M117" t="inlineStr"/>
       <c r="N117" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="O117" t="n">
         <v>0</v>
@@ -4918,7 +4918,7 @@
         <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="H122" t="inlineStr"/>
       <c r="I122" t="inlineStr"/>
@@ -4998,7 +4998,7 @@
         <v>0</v>
       </c>
       <c r="M124" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="N124" t="inlineStr"/>
       <c r="O124" t="inlineStr"/>
@@ -5018,7 +5018,7 @@
       <c r="F125" t="inlineStr"/>
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="I125" t="inlineStr"/>
       <c r="J125" t="inlineStr"/>
@@ -5026,7 +5026,7 @@
       <c r="L125" t="inlineStr"/>
       <c r="M125" t="inlineStr"/>
       <c r="N125" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="O125" t="n">
         <v>0</v>
@@ -5099,7 +5099,7 @@
         <v>0</v>
       </c>
       <c r="G127" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="H127" t="inlineStr"/>
       <c r="I127" t="inlineStr"/>
@@ -5140,7 +5140,7 @@
         <v>0</v>
       </c>
       <c r="M128" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="N128" t="inlineStr"/>
       <c r="O128" t="inlineStr"/>
@@ -5160,7 +5160,7 @@
       <c r="F129" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="I129" t="inlineStr"/>
       <c r="J129" t="inlineStr"/>
@@ -5168,7 +5168,7 @@
       <c r="L129" t="inlineStr"/>
       <c r="M129" t="inlineStr"/>
       <c r="N129" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="O129" t="n">
         <v>0</v>
@@ -5202,7 +5202,7 @@
         <v>0</v>
       </c>
       <c r="G130" t="n">
-        <v>1120772.8</v>
+        <v>2254850.14</v>
       </c>
       <c r="H130" t="inlineStr"/>
       <c r="I130" t="inlineStr"/>
@@ -5282,7 +5282,7 @@
         <v>0</v>
       </c>
       <c r="M132" t="n">
-        <v>1120772.8</v>
+        <v>2254850.14</v>
       </c>
       <c r="N132" t="inlineStr"/>
       <c r="O132" t="inlineStr"/>
@@ -5302,7 +5302,7 @@
       <c r="F133" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="n">
-        <v>1120772.8</v>
+        <v>2254850.14</v>
       </c>
       <c r="I133" t="inlineStr"/>
       <c r="J133" t="inlineStr"/>
@@ -5310,7 +5310,7 @@
       <c r="L133" t="inlineStr"/>
       <c r="M133" t="inlineStr"/>
       <c r="N133" t="n">
-        <v>1120772.8</v>
+        <v>2254850.14</v>
       </c>
       <c r="O133" t="n">
         <v>0</v>
@@ -5344,7 +5344,7 @@
         <v>0</v>
       </c>
       <c r="G134" t="n">
-        <v>22324.2</v>
+        <v>46094.97</v>
       </c>
       <c r="H134" t="inlineStr"/>
       <c r="I134" t="inlineStr"/>
@@ -5424,7 +5424,7 @@
         <v>0</v>
       </c>
       <c r="M136" t="n">
-        <v>867227.2</v>
+        <v>244149.86</v>
       </c>
       <c r="N136" t="inlineStr"/>
       <c r="O136" t="inlineStr"/>
@@ -5459,7 +5459,7 @@
         <v>1</v>
       </c>
       <c r="M137" t="n">
-        <v>-844903</v>
+        <v>-198054.89</v>
       </c>
       <c r="N137" t="inlineStr"/>
       <c r="O137" t="inlineStr"/>
@@ -5479,7 +5479,7 @@
       <c r="F138" t="inlineStr"/>
       <c r="G138" t="inlineStr"/>
       <c r="H138" t="n">
-        <v>22324.2</v>
+        <v>46094.97</v>
       </c>
       <c r="I138" t="inlineStr"/>
       <c r="J138" t="inlineStr"/>
@@ -5487,7 +5487,7 @@
       <c r="L138" t="inlineStr"/>
       <c r="M138" t="inlineStr"/>
       <c r="N138" t="n">
-        <v>22324.19999999995</v>
+        <v>46094.96999999997</v>
       </c>
       <c r="O138" t="n">
         <v>0</v>
@@ -5521,7 +5521,7 @@
         <v>0</v>
       </c>
       <c r="G139" t="n">
-        <v>22324.2</v>
+        <v>46094.97</v>
       </c>
       <c r="H139" t="inlineStr"/>
       <c r="I139" t="inlineStr"/>
@@ -5601,7 +5601,7 @@
         <v>0</v>
       </c>
       <c r="M141" t="n">
-        <v>867227.2</v>
+        <v>244149.86</v>
       </c>
       <c r="N141" t="inlineStr"/>
       <c r="O141" t="inlineStr"/>
@@ -5636,7 +5636,7 @@
         <v>1</v>
       </c>
       <c r="M142" t="n">
-        <v>-844903</v>
+        <v>-198054.89</v>
       </c>
       <c r="N142" t="inlineStr"/>
       <c r="O142" t="inlineStr"/>
@@ -5656,7 +5656,7 @@
       <c r="F143" t="inlineStr"/>
       <c r="G143" t="inlineStr"/>
       <c r="H143" t="n">
-        <v>22324.2</v>
+        <v>46094.97</v>
       </c>
       <c r="I143" t="inlineStr"/>
       <c r="J143" t="inlineStr"/>
@@ -5664,7 +5664,7 @@
       <c r="L143" t="inlineStr"/>
       <c r="M143" t="inlineStr"/>
       <c r="N143" t="n">
-        <v>22324.19999999995</v>
+        <v>46094.96999999997</v>
       </c>
       <c r="O143" t="n">
         <v>0</v>
@@ -5698,7 +5698,7 @@
         <v>0</v>
       </c>
       <c r="G144" t="n">
-        <v>17785.11</v>
+        <v>10043.6</v>
       </c>
       <c r="H144" t="inlineStr"/>
       <c r="I144" t="inlineStr"/>
@@ -5778,7 +5778,7 @@
         <v>0</v>
       </c>
       <c r="M146" t="n">
-        <v>844903</v>
+        <v>198054.89</v>
       </c>
       <c r="N146" t="inlineStr"/>
       <c r="O146" t="inlineStr"/>
@@ -5813,7 +5813,7 @@
         <v>1</v>
       </c>
       <c r="M147" t="n">
-        <v>-827117.89</v>
+        <v>-188011.29</v>
       </c>
       <c r="N147" t="inlineStr"/>
       <c r="O147" t="inlineStr"/>
@@ -5833,7 +5833,7 @@
       <c r="F148" t="inlineStr"/>
       <c r="G148" t="inlineStr"/>
       <c r="H148" t="n">
-        <v>17785.11</v>
+        <v>10043.6</v>
       </c>
       <c r="I148" t="inlineStr"/>
       <c r="J148" t="inlineStr"/>
@@ -5841,10 +5841,10 @@
       <c r="L148" t="inlineStr"/>
       <c r="M148" t="inlineStr"/>
       <c r="N148" t="n">
-        <v>17785.10999999999</v>
+        <v>10043.60000000001</v>
       </c>
       <c r="O148" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="149">
@@ -5875,7 +5875,7 @@
         <v>0</v>
       </c>
       <c r="G149" t="n">
-        <v>17785.11</v>
+        <v>10043.6</v>
       </c>
       <c r="H149" t="inlineStr"/>
       <c r="I149" t="inlineStr"/>
@@ -5955,7 +5955,7 @@
         <v>0</v>
       </c>
       <c r="M151" t="n">
-        <v>844903</v>
+        <v>198054.89</v>
       </c>
       <c r="N151" t="inlineStr"/>
       <c r="O151" t="inlineStr"/>
@@ -5990,7 +5990,7 @@
         <v>1</v>
       </c>
       <c r="M152" t="n">
-        <v>-827117.89</v>
+        <v>-188011.29</v>
       </c>
       <c r="N152" t="inlineStr"/>
       <c r="O152" t="inlineStr"/>
@@ -6010,7 +6010,7 @@
       <c r="F153" t="inlineStr"/>
       <c r="G153" t="inlineStr"/>
       <c r="H153" t="n">
-        <v>17785.11</v>
+        <v>10043.6</v>
       </c>
       <c r="I153" t="inlineStr"/>
       <c r="J153" t="inlineStr"/>
@@ -6018,10 +6018,10 @@
       <c r="L153" t="inlineStr"/>
       <c r="M153" t="inlineStr"/>
       <c r="N153" t="n">
-        <v>17785.10999999999</v>
+        <v>10043.60000000001</v>
       </c>
       <c r="O153" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="154">
@@ -6052,7 +6052,7 @@
         <v>0</v>
       </c>
       <c r="G154" t="n">
-        <v>827117.89</v>
+        <v>188011.29</v>
       </c>
       <c r="H154" t="inlineStr"/>
       <c r="I154" t="inlineStr"/>
@@ -6132,7 +6132,7 @@
         <v>0</v>
       </c>
       <c r="M156" t="n">
-        <v>827117.89</v>
+        <v>188011.29</v>
       </c>
       <c r="N156" t="inlineStr"/>
       <c r="O156" t="inlineStr"/>
@@ -6152,7 +6152,7 @@
       <c r="F157" t="inlineStr"/>
       <c r="G157" t="inlineStr"/>
       <c r="H157" t="n">
-        <v>827117.89</v>
+        <v>188011.29</v>
       </c>
       <c r="I157" t="inlineStr"/>
       <c r="J157" t="inlineStr"/>
@@ -6160,7 +6160,7 @@
       <c r="L157" t="inlineStr"/>
       <c r="M157" t="inlineStr"/>
       <c r="N157" t="n">
-        <v>827117.89</v>
+        <v>188011.29</v>
       </c>
       <c r="O157" t="n">
         <v>0</v>
@@ -6194,7 +6194,7 @@
         <v>0</v>
       </c>
       <c r="G158" t="n">
-        <v>827117.89</v>
+        <v>188011.29</v>
       </c>
       <c r="H158" t="inlineStr"/>
       <c r="I158" t="inlineStr"/>
@@ -6274,7 +6274,7 @@
         <v>0</v>
       </c>
       <c r="M160" t="n">
-        <v>827117.89</v>
+        <v>188011.29</v>
       </c>
       <c r="N160" t="inlineStr"/>
       <c r="O160" t="inlineStr"/>
@@ -6294,7 +6294,7 @@
       <c r="F161" t="inlineStr"/>
       <c r="G161" t="inlineStr"/>
       <c r="H161" t="n">
-        <v>827117.89</v>
+        <v>188011.29</v>
       </c>
       <c r="I161" t="inlineStr"/>
       <c r="J161" t="inlineStr"/>
@@ -6302,7 +6302,7 @@
       <c r="L161" t="inlineStr"/>
       <c r="M161" t="inlineStr"/>
       <c r="N161" t="n">
-        <v>827117.89</v>
+        <v>188011.29</v>
       </c>
       <c r="O161" t="n">
         <v>0</v>
@@ -6620,7 +6620,7 @@
         <v>0</v>
       </c>
       <c r="G170" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="H170" t="inlineStr"/>
       <c r="I170" t="inlineStr"/>
@@ -6700,7 +6700,7 @@
         <v>0</v>
       </c>
       <c r="M172" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="N172" t="inlineStr"/>
       <c r="O172" t="inlineStr"/>
@@ -6720,7 +6720,7 @@
       <c r="F173" t="inlineStr"/>
       <c r="G173" t="inlineStr"/>
       <c r="H173" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr"/>
@@ -6728,7 +6728,7 @@
       <c r="L173" t="inlineStr"/>
       <c r="M173" t="inlineStr"/>
       <c r="N173" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="O173" t="n">
         <v>0</v>
@@ -6904,7 +6904,7 @@
         <v>0</v>
       </c>
       <c r="G178" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="H178" t="inlineStr"/>
       <c r="I178" t="inlineStr"/>
@@ -6984,7 +6984,7 @@
         <v>0</v>
       </c>
       <c r="M180" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="N180" t="inlineStr"/>
       <c r="O180" t="inlineStr"/>
@@ -7004,7 +7004,7 @@
       <c r="F181" t="inlineStr"/>
       <c r="G181" t="inlineStr"/>
       <c r="H181" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="I181" t="inlineStr"/>
       <c r="J181" t="inlineStr"/>
@@ -7012,7 +7012,7 @@
       <c r="L181" t="inlineStr"/>
       <c r="M181" t="inlineStr"/>
       <c r="N181" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="O181" t="n">
         <v>0</v>
@@ -7743,7 +7743,7 @@
         <v>0</v>
       </c>
       <c r="G201" t="n">
-        <v>2040000</v>
+        <v>2499000</v>
       </c>
       <c r="H201" t="inlineStr"/>
       <c r="I201" t="inlineStr"/>
@@ -7782,7 +7782,7 @@
         <v>1</v>
       </c>
       <c r="G202" t="n">
-        <v>-52000</v>
+        <v>-0</v>
       </c>
       <c r="H202" t="inlineStr"/>
       <c r="I202" t="inlineStr"/>
@@ -7827,7 +7827,7 @@
         <v>0</v>
       </c>
       <c r="M203" t="n">
-        <v>1988000</v>
+        <v>2499000</v>
       </c>
       <c r="N203" t="inlineStr"/>
       <c r="O203" t="inlineStr"/>
@@ -7886,7 +7886,7 @@
       <c r="F205" t="inlineStr"/>
       <c r="G205" t="inlineStr"/>
       <c r="H205" t="n">
-        <v>1988000</v>
+        <v>2499000</v>
       </c>
       <c r="I205" t="inlineStr"/>
       <c r="J205" t="inlineStr"/>
@@ -7894,7 +7894,7 @@
       <c r="L205" t="inlineStr"/>
       <c r="M205" t="inlineStr"/>
       <c r="N205" t="n">
-        <v>1988000</v>
+        <v>2499000</v>
       </c>
       <c r="O205" t="n">
         <v>0</v>
@@ -8298,7 +8298,7 @@
         <v>0</v>
       </c>
       <c r="G216" t="n">
-        <v>875812.13</v>
+        <v>244149.86</v>
       </c>
       <c r="H216" t="inlineStr"/>
       <c r="I216" t="inlineStr"/>
@@ -8337,7 +8337,7 @@
         <v>1</v>
       </c>
       <c r="G217" t="n">
-        <v>-8584.93</v>
+        <v>-0</v>
       </c>
       <c r="H217" t="inlineStr"/>
       <c r="I217" t="inlineStr"/>
@@ -8382,7 +8382,7 @@
         <v>0</v>
       </c>
       <c r="M218" t="n">
-        <v>867227.2</v>
+        <v>244149.86</v>
       </c>
       <c r="N218" t="inlineStr"/>
       <c r="O218" t="inlineStr"/>
@@ -8441,7 +8441,7 @@
       <c r="F220" t="inlineStr"/>
       <c r="G220" t="inlineStr"/>
       <c r="H220" t="n">
-        <v>867227.2</v>
+        <v>244149.86</v>
       </c>
       <c r="I220" t="inlineStr"/>
       <c r="J220" t="inlineStr"/>
@@ -8449,7 +8449,7 @@
       <c r="L220" t="inlineStr"/>
       <c r="M220" t="inlineStr"/>
       <c r="N220" t="n">
-        <v>867227.2</v>
+        <v>244149.86</v>
       </c>
       <c r="O220" t="n">
         <v>0</v>
@@ -8483,7 +8483,7 @@
         <v>0</v>
       </c>
       <c r="G221" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="H221" t="inlineStr"/>
       <c r="I221" t="inlineStr"/>
@@ -8567,7 +8567,7 @@
         <v>0</v>
       </c>
       <c r="M223" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="N223" t="inlineStr"/>
       <c r="O223" t="inlineStr"/>
@@ -8626,7 +8626,7 @@
       <c r="F225" t="inlineStr"/>
       <c r="G225" t="inlineStr"/>
       <c r="H225" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="I225" t="inlineStr"/>
       <c r="J225" t="inlineStr"/>
@@ -8634,7 +8634,7 @@
       <c r="L225" t="inlineStr"/>
       <c r="M225" t="inlineStr"/>
       <c r="N225" t="n">
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="O225" t="n">
         <v>0</v>
@@ -8668,7 +8668,7 @@
         <v>0</v>
       </c>
       <c r="G226" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="H226" t="inlineStr"/>
       <c r="I226" t="inlineStr"/>
@@ -8752,7 +8752,7 @@
         <v>0</v>
       </c>
       <c r="M228" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="N228" t="inlineStr"/>
       <c r="O228" t="inlineStr"/>
@@ -8811,7 +8811,7 @@
       <c r="F230" t="inlineStr"/>
       <c r="G230" t="inlineStr"/>
       <c r="H230" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="I230" t="inlineStr"/>
       <c r="J230" t="inlineStr"/>
@@ -8819,7 +8819,7 @@
       <c r="L230" t="inlineStr"/>
       <c r="M230" t="inlineStr"/>
       <c r="N230" t="n">
-        <v>9814.9</v>
+        <v>0</v>
       </c>
       <c r="O230" t="n">
         <v>0</v>
@@ -21063,7 +21063,7 @@
         <v>0</v>
       </c>
       <c r="G561" t="n">
-        <v>81223.58</v>
+        <v>27600.83</v>
       </c>
       <c r="H561" t="inlineStr"/>
       <c r="I561" t="inlineStr"/>
@@ -21147,7 +21147,7 @@
         <v>0</v>
       </c>
       <c r="M563" t="n">
-        <v>81223.58</v>
+        <v>27600.83</v>
       </c>
       <c r="N563" t="inlineStr"/>
       <c r="O563" t="inlineStr"/>
@@ -21206,7 +21206,7 @@
       <c r="F565" t="inlineStr"/>
       <c r="G565" t="inlineStr"/>
       <c r="H565" t="n">
-        <v>81223.58</v>
+        <v>27600.83</v>
       </c>
       <c r="I565" t="inlineStr"/>
       <c r="J565" t="inlineStr"/>
@@ -21214,7 +21214,7 @@
       <c r="L565" t="inlineStr"/>
       <c r="M565" t="inlineStr"/>
       <c r="N565" t="n">
-        <v>81223.58</v>
+        <v>27600.83</v>
       </c>
       <c r="O565" t="n">
         <v>0</v>
@@ -25133,7 +25133,7 @@
         <v>0</v>
       </c>
       <c r="G671" t="n">
-        <v>1314362.2</v>
+        <v>413341.85</v>
       </c>
       <c r="H671" t="inlineStr"/>
       <c r="I671" t="inlineStr"/>
@@ -25217,7 +25217,7 @@
         <v>0</v>
       </c>
       <c r="M673" t="n">
-        <v>1314362.2</v>
+        <v>413341.85</v>
       </c>
       <c r="N673" t="inlineStr"/>
       <c r="O673" t="inlineStr"/>
@@ -25276,7 +25276,7 @@
       <c r="F675" t="inlineStr"/>
       <c r="G675" t="inlineStr"/>
       <c r="H675" t="n">
-        <v>1314362.2</v>
+        <v>413341.85</v>
       </c>
       <c r="I675" t="inlineStr"/>
       <c r="J675" t="inlineStr"/>
@@ -25284,7 +25284,7 @@
       <c r="L675" t="inlineStr"/>
       <c r="M675" t="inlineStr"/>
       <c r="N675" t="n">
-        <v>1314362.2</v>
+        <v>413341.85</v>
       </c>
       <c r="O675" t="n">
         <v>0</v>
@@ -32348,7 +32348,7 @@
         <v>0</v>
       </c>
       <c r="G866" t="n">
-        <v>500.06</v>
+        <v>0</v>
       </c>
       <c r="H866" t="inlineStr"/>
       <c r="I866" t="inlineStr"/>
@@ -32432,7 +32432,7 @@
         <v>0</v>
       </c>
       <c r="M868" t="n">
-        <v>500.06</v>
+        <v>0</v>
       </c>
       <c r="N868" t="inlineStr"/>
       <c r="O868" t="inlineStr"/>
@@ -32491,7 +32491,7 @@
       <c r="F870" t="inlineStr"/>
       <c r="G870" t="inlineStr"/>
       <c r="H870" t="n">
-        <v>500.06</v>
+        <v>0</v>
       </c>
       <c r="I870" t="inlineStr"/>
       <c r="J870" t="inlineStr"/>
@@ -32499,7 +32499,7 @@
       <c r="L870" t="inlineStr"/>
       <c r="M870" t="inlineStr"/>
       <c r="N870" t="n">
-        <v>500.06</v>
+        <v>0</v>
       </c>
       <c r="O870" t="n">
         <v>0</v>
@@ -33828,7 +33828,7 @@
         <v>0</v>
       </c>
       <c r="G906" t="n">
-        <v>516.26</v>
+        <v>0</v>
       </c>
       <c r="H906" t="inlineStr"/>
       <c r="I906" t="inlineStr"/>
@@ -33912,7 +33912,7 @@
         <v>0</v>
       </c>
       <c r="M908" t="n">
-        <v>516.26</v>
+        <v>0</v>
       </c>
       <c r="N908" t="inlineStr"/>
       <c r="O908" t="inlineStr"/>
@@ -33971,7 +33971,7 @@
       <c r="F910" t="inlineStr"/>
       <c r="G910" t="inlineStr"/>
       <c r="H910" t="n">
-        <v>516.26</v>
+        <v>0</v>
       </c>
       <c r="I910" t="inlineStr"/>
       <c r="J910" t="inlineStr"/>
@@ -33979,7 +33979,7 @@
       <c r="L910" t="inlineStr"/>
       <c r="M910" t="inlineStr"/>
       <c r="N910" t="n">
-        <v>516.26</v>
+        <v>0</v>
       </c>
       <c r="O910" t="n">
         <v>0</v>
@@ -34753,7 +34753,7 @@
         <v>0</v>
       </c>
       <c r="G931" t="n">
-        <v>1314362.2</v>
+        <v>413341.85</v>
       </c>
       <c r="H931" t="inlineStr"/>
       <c r="I931" t="inlineStr"/>
@@ -34831,7 +34831,7 @@
         <v>1</v>
       </c>
       <c r="G933" t="n">
-        <v>-839086.95</v>
+        <v>-188053.58</v>
       </c>
       <c r="H933" t="inlineStr"/>
       <c r="I933" t="inlineStr"/>
@@ -34915,7 +34915,7 @@
         <v>0</v>
       </c>
       <c r="M935" t="n">
-        <v>475275.25</v>
+        <v>225288.27</v>
       </c>
       <c r="N935" t="inlineStr"/>
       <c r="O935" t="inlineStr"/>
@@ -35052,7 +35052,7 @@
       <c r="F939" t="inlineStr"/>
       <c r="G939" t="inlineStr"/>
       <c r="H939" t="n">
-        <v>475275.25</v>
+        <v>225288.27</v>
       </c>
       <c r="I939" t="inlineStr"/>
       <c r="J939" t="inlineStr"/>
@@ -35060,7 +35060,7 @@
       <c r="L939" t="inlineStr"/>
       <c r="M939" t="inlineStr"/>
       <c r="N939" t="n">
-        <v>475275.25</v>
+        <v>225288.27</v>
       </c>
       <c r="O939" t="n">
         <v>0</v>
@@ -35094,7 +35094,7 @@
         <v>0</v>
       </c>
       <c r="G940" t="n">
-        <v>435165.94</v>
+        <v>169149.7</v>
       </c>
       <c r="H940" t="inlineStr"/>
       <c r="I940" t="inlineStr"/>
@@ -35178,7 +35178,7 @@
         <v>0</v>
       </c>
       <c r="M942" t="n">
-        <v>475275.25</v>
+        <v>225288.27</v>
       </c>
       <c r="N942" t="inlineStr"/>
       <c r="O942" t="inlineStr"/>
@@ -35256,7 +35256,7 @@
         <v>1</v>
       </c>
       <c r="M944" t="n">
-        <v>-17785.11</v>
+        <v>-10043.6</v>
       </c>
       <c r="N944" t="inlineStr"/>
       <c r="O944" t="inlineStr"/>
@@ -35412,7 +35412,7 @@
         <v>1</v>
       </c>
       <c r="M948" t="n">
-        <v>-22324.2</v>
+        <v>-46094.97</v>
       </c>
       <c r="N948" t="inlineStr"/>
       <c r="O948" t="inlineStr"/>
@@ -35471,7 +35471,7 @@
       <c r="F950" t="inlineStr"/>
       <c r="G950" t="inlineStr"/>
       <c r="H950" t="n">
-        <v>435165.94</v>
+        <v>169149.7</v>
       </c>
       <c r="I950" t="inlineStr"/>
       <c r="J950" t="inlineStr"/>
@@ -35479,7 +35479,7 @@
       <c r="L950" t="inlineStr"/>
       <c r="M950" t="inlineStr"/>
       <c r="N950" t="n">
-        <v>435165.94</v>
+        <v>169149.7</v>
       </c>
       <c r="O950" t="n">
         <v>0</v>
@@ -35513,7 +35513,7 @@
         <v>0</v>
       </c>
       <c r="G951" t="n">
-        <v>1658334.89</v>
+        <v>2490886.59</v>
       </c>
       <c r="H951" t="inlineStr"/>
       <c r="I951" t="inlineStr"/>
@@ -35552,7 +35552,7 @@
         <v>1</v>
       </c>
       <c r="G952" t="n">
-        <v>-53141.1</v>
+        <v>-58843.64</v>
       </c>
       <c r="H952" t="inlineStr"/>
       <c r="I952" t="inlineStr"/>
@@ -35591,7 +35591,7 @@
         <v>0</v>
       </c>
       <c r="G953" t="n">
-        <v>2181143.85</v>
+        <v>3457928.48</v>
       </c>
       <c r="H953" t="inlineStr"/>
       <c r="I953" t="inlineStr"/>
@@ -35630,7 +35630,7 @@
         <v>1</v>
       </c>
       <c r="G954" t="n">
-        <v>-2305626.18</v>
+        <v>-3591792.61</v>
       </c>
       <c r="H954" t="inlineStr"/>
       <c r="I954" t="inlineStr"/>
@@ -35675,7 +35675,7 @@
         <v>0</v>
       </c>
       <c r="M955" t="n">
-        <v>3489872.25</v>
+        <v>2912299.56</v>
       </c>
       <c r="N955" t="inlineStr"/>
       <c r="O955" t="inlineStr"/>
@@ -35792,7 +35792,7 @@
         <v>1</v>
       </c>
       <c r="M958" t="n">
-        <v>-2009160.79</v>
+        <v>-614120.74</v>
       </c>
       <c r="N958" t="inlineStr"/>
       <c r="O958" t="inlineStr"/>
@@ -35812,7 +35812,7 @@
       <c r="F959" t="inlineStr"/>
       <c r="G959" t="inlineStr"/>
       <c r="H959" t="n">
-        <v>1480711.459999999</v>
+        <v>2298178.82</v>
       </c>
       <c r="I959" t="inlineStr"/>
       <c r="J959" t="inlineStr"/>
@@ -35820,7 +35820,7 @@
       <c r="L959" t="inlineStr"/>
       <c r="M959" t="inlineStr"/>
       <c r="N959" t="n">
-        <v>1480711.46</v>
+        <v>2298178.82</v>
       </c>
       <c r="O959" t="n">
         <v>-0</v>
@@ -35854,7 +35854,7 @@
         <v>0</v>
       </c>
       <c r="G960" t="n">
-        <v>435165.94</v>
+        <v>169149.7</v>
       </c>
       <c r="H960" t="inlineStr"/>
       <c r="I960" t="inlineStr"/>
@@ -35938,7 +35938,7 @@
         <v>0</v>
       </c>
       <c r="M962" t="n">
-        <v>11384.9</v>
+        <v>0</v>
       </c>
       <c r="N962" t="inlineStr"/>
       <c r="O962" t="inlineStr"/>
@@ -36016,7 +36016,7 @@
         <v>1</v>
       </c>
       <c r="M964" t="n">
-        <v>-9814.9</v>
+        <v>-0</v>
       </c>
       <c r="N964" t="inlineStr"/>
       <c r="O964" t="inlineStr"/>
@@ -36172,7 +36172,7 @@
         <v>1</v>
       </c>
       <c r="M968" t="n">
-        <v>-1570</v>
+        <v>-0</v>
       </c>
       <c r="N968" t="inlineStr"/>
       <c r="O968" t="inlineStr"/>
@@ -36250,7 +36250,7 @@
         <v>0</v>
       </c>
       <c r="M970" t="n">
-        <v>1302393.14</v>
+        <v>413299.56</v>
       </c>
       <c r="N970" t="inlineStr"/>
       <c r="O970" t="inlineStr"/>
@@ -36441,7 +36441,7 @@
         <v>1</v>
       </c>
       <c r="M975" t="n">
-        <v>-867227.2</v>
+        <v>-244149.86</v>
       </c>
       <c r="N975" t="inlineStr"/>
       <c r="O975" t="inlineStr"/>
@@ -36765,7 +36765,7 @@
       <c r="F984" t="inlineStr"/>
       <c r="G984" t="inlineStr"/>
       <c r="H984" t="n">
-        <v>435165.94</v>
+        <v>169149.7</v>
       </c>
       <c r="I984" t="inlineStr"/>
       <c r="J984" t="inlineStr"/>
@@ -36773,7 +36773,7 @@
       <c r="L984" t="inlineStr"/>
       <c r="M984" t="inlineStr"/>
       <c r="N984" t="n">
-        <v>435165.9399999999</v>
+        <v>169149.7</v>
       </c>
       <c r="O984" t="n">
         <v>0</v>
@@ -36807,7 +36807,7 @@
         <v>0</v>
       </c>
       <c r="G985" t="n">
-        <v>435165.94</v>
+        <v>169149.7</v>
       </c>
       <c r="H985" t="inlineStr"/>
       <c r="I985" t="inlineStr"/>
@@ -36891,7 +36891,7 @@
         <v>0</v>
       </c>
       <c r="M987" t="n">
-        <v>475275.25</v>
+        <v>225288.27</v>
       </c>
       <c r="N987" t="inlineStr"/>
       <c r="O987" t="inlineStr"/>
@@ -36969,7 +36969,7 @@
         <v>1</v>
       </c>
       <c r="M989" t="n">
-        <v>-17785.11</v>
+        <v>-10043.6</v>
       </c>
       <c r="N989" t="inlineStr"/>
       <c r="O989" t="inlineStr"/>
@@ -37125,7 +37125,7 @@
         <v>1</v>
       </c>
       <c r="M993" t="n">
-        <v>-22324.2</v>
+        <v>-46094.97</v>
       </c>
       <c r="N993" t="inlineStr"/>
       <c r="O993" t="inlineStr"/>
@@ -37184,7 +37184,7 @@
       <c r="F995" t="inlineStr"/>
       <c r="G995" t="inlineStr"/>
       <c r="H995" t="n">
-        <v>435165.94</v>
+        <v>169149.7</v>
       </c>
       <c r="I995" t="inlineStr"/>
       <c r="J995" t="inlineStr"/>
@@ -37192,7 +37192,7 @@
       <c r="L995" t="inlineStr"/>
       <c r="M995" t="inlineStr"/>
       <c r="N995" t="n">
-        <v>435165.94</v>
+        <v>169149.7</v>
       </c>
       <c r="O995" t="n">
         <v>0</v>
@@ -37226,7 +37226,7 @@
         <v>0</v>
       </c>
       <c r="G996" t="n">
-        <v>22324.2</v>
+        <v>46094.97</v>
       </c>
       <c r="H996" t="inlineStr"/>
       <c r="I996" t="inlineStr"/>
@@ -37310,7 +37310,7 @@
         <v>0</v>
       </c>
       <c r="M998" t="n">
-        <v>22324.2</v>
+        <v>46094.97</v>
       </c>
       <c r="N998" t="inlineStr"/>
       <c r="O998" t="inlineStr"/>
@@ -37447,7 +37447,7 @@
       <c r="F1002" t="inlineStr"/>
       <c r="G1002" t="inlineStr"/>
       <c r="H1002" t="n">
-        <v>22324.2</v>
+        <v>46094.97</v>
       </c>
       <c r="I1002" t="inlineStr"/>
       <c r="J1002" t="inlineStr"/>
@@ -37455,7 +37455,7 @@
       <c r="L1002" t="inlineStr"/>
       <c r="M1002" t="inlineStr"/>
       <c r="N1002" t="n">
-        <v>22324.2</v>
+        <v>46094.97</v>
       </c>
       <c r="O1002" t="n">
         <v>0</v>
@@ -37489,7 +37489,7 @@
         <v>0</v>
       </c>
       <c r="G1003" t="n">
-        <v>17785.11</v>
+        <v>10043.6</v>
       </c>
       <c r="H1003" t="inlineStr"/>
       <c r="I1003" t="inlineStr"/>
@@ -37573,7 +37573,7 @@
         <v>0</v>
       </c>
       <c r="M1005" t="n">
-        <v>17785.11</v>
+        <v>10043.6</v>
       </c>
       <c r="N1005" t="inlineStr"/>
       <c r="O1005" t="inlineStr"/>
@@ -37944,7 +37944,7 @@
       <c r="F1015" t="inlineStr"/>
       <c r="G1015" t="inlineStr"/>
       <c r="H1015" t="n">
-        <v>17785.11</v>
+        <v>10043.6</v>
       </c>
       <c r="I1015" t="inlineStr"/>
       <c r="J1015" t="inlineStr"/>
@@ -37952,7 +37952,7 @@
       <c r="L1015" t="inlineStr"/>
       <c r="M1015" t="inlineStr"/>
       <c r="N1015" t="n">
-        <v>17785.11</v>
+        <v>10043.6</v>
       </c>
       <c r="O1015" t="n">
         <v>0</v>

</xml_diff>